<commit_message>
PO002 web service PR PO
</commit_message>
<xml_diff>
--- a/XCustPr/doc/60-11-13/RD_CUSTOMIZATION_PLAN_V02R00.xlsx
+++ b/XCustPr/doc/60-11-13/RD_CUSTOMIZATION_PLAN_V02R00.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekapop\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\ice\XCustPr\XCustPr\doc\60-11-13\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -226,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +266,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -375,6 +381,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,7 +665,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1083,8 +1090,8 @@
       <c r="J16" s="13">
         <v>43057</v>
       </c>
-      <c r="K16" s="13">
-        <v>43057</v>
+      <c r="K16" s="27">
+        <v>43061</v>
       </c>
       <c r="L16" s="16" t="s">
         <v>56</v>
@@ -1121,8 +1128,8 @@
       <c r="J17" s="13">
         <v>43057</v>
       </c>
-      <c r="K17" s="13">
-        <v>43057</v>
+      <c r="K17" s="27">
+        <v>43059</v>
       </c>
       <c r="L17" s="16" t="s">
         <v>56</v>
@@ -1197,8 +1204,8 @@
       <c r="J19" s="13">
         <v>43052</v>
       </c>
-      <c r="K19" s="13">
-        <v>43052</v>
+      <c r="K19" s="27">
+        <v>43059</v>
       </c>
       <c r="L19" s="16" t="s">
         <v>56</v>

</xml_diff>